<commit_message>
Add query execution time calculation
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -528,11 +528,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>45_YATAFENE</t>
+          <t>30_AIT BOUMEHDI</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -550,11 +550,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>26_M'KIRA</t>
+          <t>37_AZZEFOUN</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
@@ -572,11 +572,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>63_IMSOUHAL</t>
+          <t>12_BOUNOUH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -594,11 +594,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>41_IFIGHA</t>
+          <t>60_IBOUDRAREN</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -616,11 +616,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>04_FREHA</t>
+          <t>65_AIT BOUADDOU</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -638,11 +638,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>34_BOUZGUEN</t>
+          <t>44_AKERROU</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
@@ -660,11 +660,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>36_OUADHIA</t>
+          <t>54_IFLISSEN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
@@ -682,11 +682,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>15_BENI AISSI</t>
+          <t>46_BENI ZIKI</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -704,11 +704,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>56_AIT YAHIA MOU,</t>
+          <t>36_OUADHIA</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>293</v>
+        <v>50</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -726,11 +726,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>25_AIN ZAOUIA</t>
+          <t>15_BENI AISSI</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -748,11 +748,11 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>38_TIGZIRT</t>
+          <t>56_AIT YAHIA MOU,</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>40</v>
+        <v>293</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -770,11 +770,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>59_SIDI NAAMANE</t>
+          <t>25_AIN ZAOUIA</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
@@ -792,11 +792,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>51_TIZI N'THLATA</t>
+          <t>38_TIGZIRT</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>103</v>
+        <v>40</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -814,11 +814,11 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>48_OUACIF</t>
+          <t>45_YATAFENE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
@@ -836,11 +836,11 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>08_TIMIZART</t>
+          <t>26_M'KIRA</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>158</v>
+        <v>94</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -858,11 +858,11 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>24_OUAGUENOUN</t>
+          <t>63_IMSOUHAL</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -880,11 +880,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>47_DRAA BEN KHEDA</t>
+          <t>41_IFIGHA</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -902,11 +902,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>30_AIT BOUMEHDI</t>
+          <t>04_FREHA</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -924,11 +924,11 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>37_AZZEFOUN</t>
+          <t>34_BOUZGUEN</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -946,11 +946,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>12_BOUNOUH</t>
+          <t>59_SIDI NAAMANE</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
@@ -968,11 +968,11 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>60_IBOUDRAREN</t>
+          <t>51_TIZI N'THLATA</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
@@ -990,11 +990,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>65_AIT BOUADDOU</t>
+          <t>48_OUACIF</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
@@ -1012,11 +1012,11 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>44_AKERROU</t>
+          <t>08_TIMIZART</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
@@ -1034,11 +1034,11 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>54_IFLISSEN</t>
+          <t>24_OUAGUENOUN</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -1056,11 +1056,11 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>46_BENI ZIKI</t>
+          <t>47_DRAA BEN KHEDA</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -1078,11 +1078,11 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>21_LARBA NAIT IRATHEN</t>
+          <t>16_BENI ZMENZER</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -1100,11 +1100,11 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>10_DRAA EL MIZAN</t>
+          <t>09_MAKOUDA</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>100</v>
+        <v>159</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
@@ -1122,11 +1122,11 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>64_TADMAIT</t>
+          <t>53_AGHRIB</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -1144,11 +1144,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>39_DJEBEL AISSA MIMOUN</t>
+          <t>29_MAATKA</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -1166,11 +1166,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>13_AIT CHAFFAA</t>
+          <t>11_TIZI GHENIF</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
@@ -1188,11 +1188,11 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>40_BOGHNI</t>
+          <t>32_BENI DOUALA</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -1210,11 +1210,11 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>62_MIZRANA</t>
+          <t>43_TIRMIRTINE</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -1232,11 +1232,11 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>32_BENI DOUALA</t>
+          <t>52_BENI YENNI</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
@@ -1254,11 +1254,11 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>43_TIRMIRTINE</t>
+          <t>33_ILLILTEN</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>180</v>
+        <v>43</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
@@ -1276,11 +1276,11 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>14_FRIKAT</t>
+          <t>03_AKBIL</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -1298,11 +1298,11 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>67_AIT TOUDERT</t>
+          <t>27_AIT YAHIA</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -1320,11 +1320,11 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>49_IDJEUR</t>
+          <t>07_IRDJEN</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -1342,11 +1342,11 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>52_BENI YENNI</t>
+          <t>18_AZAZGA</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -1364,11 +1364,11 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>33_ILLILTEN</t>
+          <t>28_AIT MAHMOUD</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -1386,11 +1386,11 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>03_AKBIL</t>
+          <t>61_AGHNI GOUGHRAN</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -1408,11 +1408,11 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>27_AIT YAHIA</t>
+          <t>57_SOUK EL TENINE</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -1430,11 +1430,11 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>07_IRDJEN</t>
+          <t>35_AIT AGGOUACHA</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
@@ -1452,11 +1452,11 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>18_AZAZGA</t>
+          <t>19_ILOULA OUMALOU</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
@@ -1474,11 +1474,11 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>28_AIT MAHMOUD</t>
+          <t>20_YAKOUREN</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
@@ -1496,11 +1496,11 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>35_AIT AGGOUACHA</t>
+          <t>31_ABI YOUCEF</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
@@ -1518,11 +1518,11 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>19_ILOULA OUMALOU</t>
+          <t>21_LARBA NAIT IRATHEN</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -1540,11 +1540,11 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20_YAKOUREN</t>
+          <t>10_DRAA EL MIZAN</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -1562,11 +1562,11 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>31_ABI YOUCEF</t>
+          <t>64_TADMAIT</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -1584,11 +1584,11 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>01_TIZI OUZOU</t>
+          <t>39_DJEBEL AISSA MIMOUN</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
@@ -1606,11 +1606,11 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>55_BOUDJIMA</t>
+          <t>13_AIT CHAFFAA</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>116</v>
+        <v>18</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -1628,11 +1628,11 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>16_BENI ZMENZER</t>
+          <t>40_BOGHNI</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
@@ -1650,11 +1650,11 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>09_MAKOUDA</t>
+          <t>14_FRIKAT</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>159</v>
+        <v>87</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
@@ -1672,11 +1672,11 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>53_AGHRIB</t>
+          <t>67_AIT TOUDERT</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
@@ -1694,11 +1694,11 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>29_MAATKA</t>
+          <t>49_IDJEUR</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>151</v>
+        <v>70</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
@@ -1716,11 +1716,11 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>11_TIZI GHENIF</t>
+          <t>62_MIZRANA</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
@@ -1782,11 +1782,11 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>61_AGHNI GOUGHRAN</t>
+          <t>01_TIZI OUZOU</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>70</v>
+        <v>182</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
@@ -1804,11 +1804,11 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>57_SOUK EL TENINE</t>
+          <t>55_BOUDJIMA</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
@@ -1987,16 +1987,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Quinquennal 3 (2015-2019)</t>
+          <t>Quinquennal (2020 - 2024)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Programme 2016</t>
+          <t>Programme 2021</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>282</v>
+        <v>334</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2005,7 +2005,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3">
@@ -2016,11 +2016,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Programme 2021</t>
+          <t>programme 2022</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>334</v>
+        <v>802</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -2029,22 +2029,22 @@
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Quinquennal (2020 - 2024)</t>
+          <t>Quinquennal 3 (2015-2019)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>programme 2022</t>
+          <t>Programme 2016</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>802</v>
+        <v>282</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -2053,22 +2053,22 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Quinquennal 3 (2015-2019)</t>
+          <t>Quinquennal (2020 - 2024)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Programme 2015</t>
+          <t>programme 2023</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>14</v>
+        <v>1872</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -2077,22 +2077,22 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Complémentaire Quinquennal 2</t>
+          <t>Quinquennal 2 (2010-2014)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>QUINQUENNAL 2013 C</t>
+          <t>PROGRAMME Q 2014</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -2101,22 +2101,22 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>8</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Quinquennal 2 (2010-2014)</t>
+          <t>Quinquennal 3 (2015-2019)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>PQ2013</t>
+          <t>Programme  2018</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>62</v>
+        <v>431</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -2125,22 +2125,22 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>12</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Quinquennal 1 (2005-2009)</t>
+          <t>Complémentaire Quinquennal 3_</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PROGRAMME INITIAL</t>
+          <t>Complémentaire 2015</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -2149,22 +2149,22 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Quinquennal (2020 - 2024)</t>
+          <t>Quinquennal 3 (2015-2019)</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>programme 2023</t>
+          <t>Programme 2015</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1872</v>
+        <v>14</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -2173,22 +2173,22 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>55</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Quinquennal 2 (2010-2014)</t>
+          <t>Complémentaire Quinquennal 2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PROGRAMME Q 2014</t>
+          <t>QUINQUENNAL 2013 C</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -2197,22 +2197,22 @@
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>37</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PEC</t>
+          <t>Quinquennal 3 (2015-2019)</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>PROGRAMME 2002</t>
+          <t>Programme 2019</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>309</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -2221,22 +2221,22 @@
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Quinquennal 2 (2010-2014)</t>
+          <t>Quinquennal (2020 - 2024)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> QUINQUINNAL 2010</t>
+          <t>Programme 2020</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>250</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
@@ -2245,22 +2245,22 @@
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>8</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Complémentaire Quinquennal 1</t>
+          <t>Quinquennal 2 (2010-2014)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>COMPLEMENTAIRE 2009</t>
+          <t xml:space="preserve"> QUINQUENNAL 2011</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
@@ -2269,22 +2269,22 @@
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Complémentaire Quinquennal 1</t>
+          <t>Quinquennal 2 (2010-2014)</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>COMPLEMENTAIRE 2008</t>
+          <t>PQ2013</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -2293,22 +2293,22 @@
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Quinquennal (2020 - 2024)</t>
+          <t>Quinquennal 1 (2005-2009)</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Programme 2024</t>
+          <t>PROGRAMME INITIAL</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>650</v>
+        <v>25</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
@@ -2317,22 +2317,22 @@
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Complémentaire Quinquennal 2</t>
+          <t>PEC</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>QUINQUENNAL 2011C</t>
+          <t>PROGRAMME 2002</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>39</v>
+        <v>1</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
@@ -2341,22 +2341,22 @@
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Quinquennal 3 (2015-2019)</t>
+          <t>Quinquennal 2 (2010-2014)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Programme  2018</t>
+          <t xml:space="preserve"> QUINQUINNAL 2010</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>431</v>
+        <v>12</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -2365,22 +2365,22 @@
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>61</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Quinquennal (2020 - 2024)</t>
+          <t>Complémentaire Quinquennal 1</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Programme 2020</t>
+          <t>COMPLEMENTAIRE 2009</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>250</v>
+        <v>12</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -2389,22 +2389,22 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>59</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Quinquennal 2 (2010-2014)</t>
+          <t>Quinquennal (2020 - 2024)</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> QUINQUENNAL 2011</t>
+          <t>Programme 2024</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>13</v>
+        <v>650</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -2413,22 +2413,22 @@
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Complémentaire Quinquennal 3_</t>
+          <t>Complémentaire Quinquennal 2</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Complémentaire 2015</t>
+          <t>QUINQUENNAL 2011C</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -2437,22 +2437,22 @@
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Quinquennal 3 (2015-2019)</t>
+          <t>Complémentaire Quinquennal 1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Programme 2019</t>
+          <t>COMPLEMENTAIRE 2008</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>309</v>
+        <v>2</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -2461,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>60</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2586,33 +2586,33 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>60%  Deuxième Tranche</t>
+          <t>Tranche complémentaire 2</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tranche complémentaire 2</t>
+          <t>60%  Deuxième Tranche</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -2876,33 +2876,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Aménagement</t>
+          <t>Construction Nouvelle</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>5283</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Construction Nouvelle</t>
+          <t>Aménagement</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5283</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>67</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2949,7 +2949,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>00799999000784023464</t>
+          <t>A C BANQUE</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -2965,39 +2965,39 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ccp</t>
+          <t>00799999002050084924</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>00799999004049259580</t>
+          <t>CNEP</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>00799999001972781647</t>
+          <t>00799999002302028844</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -3013,7 +3013,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>00500147000000708995</t>
+          <t>00799999001282144654</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -3029,7 +3029,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>00799999002916492416</t>
+          <t>00799999000743939669</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -3045,7 +3045,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>00799999001836919082</t>
+          <t>00799999000480477290</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -3061,7 +3061,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>00799999000498448868</t>
+          <t>00799999001765015116</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -3077,7 +3077,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>00200098098100128748</t>
+          <t>00799999001894450170</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -3093,7 +3093,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>00799999002357540101</t>
+          <t>00300571012488300082</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -3109,7 +3109,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>00799999002248648483</t>
+          <t>00799999002274035323</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -3125,7 +3125,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>00799999002600087243</t>
+          <t>00799999004101159236</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -3141,39 +3141,39 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>00799999001765015116</t>
+          <t>BNA</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>00799999001894450170</t>
+          <t>BEA</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>00300571012488300082</t>
+          <t>00799999001691627438</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -3189,7 +3189,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>00799999002274035323</t>
+          <t>00799999001905721376</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -3205,17 +3205,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CCP</t>
+          <t>00799999004164827029</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1293</v>
+        <v>2</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -3237,7 +3237,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>00799999002270586197</t>
+          <t>00799999001443014595</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -3253,7 +3253,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>00799999000773086326</t>
+          <t>00799999001797480046</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -3269,7 +3269,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>00799999001346812129</t>
+          <t>00799999002495405813</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -3285,11 +3285,11 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>00799999002357767857</t>
+          <t>00799999001825091678</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
@@ -3301,7 +3301,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>00799999002496071039</t>
+          <t>00799999000264708841</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -3317,7 +3317,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>00799999000408777121</t>
+          <t>00799999001947132422</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -3333,43 +3333,43 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CNEP</t>
+          <t>00799999000784023464</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>00799999002302028844</t>
+          <t>ccp</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>00799999001282144654</t>
+          <t>00799999004049259580</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -3381,7 +3381,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>00799999000743939669</t>
+          <t>00799999001972781647</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -3397,43 +3397,43 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BDL</t>
+          <t>00799999002270586197</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CPA</t>
+          <t>00799999000773086326</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>00799999002207445890</t>
+          <t>00799999001346812129</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -3445,11 +3445,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>00799999002424922897</t>
+          <t>00799999002357767857</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -3461,7 +3461,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>00799999002651888153</t>
+          <t>00799999002496071039</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -3477,7 +3477,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>00799999002696252267</t>
+          <t>00799999000408777121</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -3493,7 +3493,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>00799999002634381981</t>
+          <t>00799999001645354170</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -3509,7 +3509,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>00799999004101159236</t>
+          <t>00799999002085623008</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -3653,39 +3653,39 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>00500147000000708995</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>BEA</t>
+          <t>00799999002916492416</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>00799999001691627438</t>
+          <t>00799999001836919082</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -3701,7 +3701,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>00799999001905721376</t>
+          <t>00799999000498448868</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -3717,11 +3717,11 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>A C BANQUE</t>
+          <t>00200098098100128748</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
@@ -3733,11 +3733,11 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>00799999002050084924</t>
+          <t>00799999002357540101</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
@@ -3749,11 +3749,11 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>00799999001443014595</t>
+          <t>00799999002248648483</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
@@ -3765,7 +3765,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>00799999001797480046</t>
+          <t>00799999002600087243</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -3781,59 +3781,59 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>00799999002495405813</t>
+          <t>CCP</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>1293</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>1</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>00799999001825091678</t>
+          <t>BDL</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>00799999000264708841</t>
+          <t>CPA</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>00799999000480477290</t>
+          <t>00799999002207445890</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
@@ -3845,7 +3845,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>00799999001947132422</t>
+          <t>00799999002424922897</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -3861,11 +3861,11 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>00799999004164827029</t>
+          <t>00799999002651888153</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
@@ -3877,7 +3877,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>00799999001645354170</t>
+          <t>00799999002696252267</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -3893,7 +3893,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>00799999002085623008</t>
+          <t>00799999002634381981</t>
         </is>
       </c>
       <c r="B61" t="n">

</xml_diff>